<commit_message>
fix pixel mapping test data
</commit_message>
<xml_diff>
--- a/application/modules/editor/testcases/editorAPI/XlfSegmentPixelLengthTest/testfiles/pixel-mapping.xlsx
+++ b/application/modules/editor/testcases/editorAPI/XlfSegmentPixelLengthTest/testfiles/pixel-mapping.xlsx
@@ -49,25 +49,7 @@
     <t xml:space="preserve">The unicodeChar column contains the decimal unicode codepoint of the represented character.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">See </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">https://en.wikipedia.org/wiki/List_of_Unicode_characters</t>
-    </r>
+    <t xml:space="preserve">See https://en.wikipedia.org/wiki/List_of_Unicode_characters</t>
   </si>
   <si>
     <t xml:space="preserve">H</t>
@@ -158,7 +140,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -169,6 +151,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -191,7 +177,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -225,7 +211,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>123</v>
+        <v>123456789</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>6</v>
@@ -248,7 +234,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>123</v>
+        <v>123456789</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>6</v>
@@ -265,13 +251,13 @@
       <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>123</v>
+        <v>123456789</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>6</v>
@@ -291,7 +277,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>123</v>
+        <v>123456789</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>6</v>
@@ -411,7 +397,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" display="https://en.wikipedia.org/wiki/List_of_Unicode_characters"/>
+    <hyperlink ref="H3" r:id="rId1" display="See https://en.wikipedia.org/wiki/List_of_Unicode_characters"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>